<commit_message>
- updated properties correspondence table for biotic elements - source code page placeholder/redirect - new url at /code/ for source code page  placeholder/redirect - new test cases - extensiveness penalty in similarity measure
</commit_message>
<xml_diff>
--- a/lcmlutils/data/correspondence/properties/LCML correction values Biotic elements properties 120.xlsx
+++ b/lcmlutils/data/correspondence/properties/LCML correction values Biotic elements properties 120.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Digre\Desktop\LCHML\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="8844"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -124,10 +129,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,11 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,26 +451,26 @@
   <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.33203125" customWidth="1"/>
     <col min="2" max="4" width="3.33203125" customWidth="1"/>
-    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
     <col min="7" max="7" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.5" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" customWidth="1"/>
     <col min="9" max="10" width="3.33203125" customWidth="1"/>
-    <col min="11" max="12" width="3.5" customWidth="1"/>
+    <col min="11" max="12" width="3.44140625" customWidth="1"/>
     <col min="13" max="13" width="3.6640625" customWidth="1"/>
     <col min="14" max="15" width="3" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" customWidth="1"/>
-    <col min="17" max="33" width="3.5" customWidth="1"/>
+    <col min="16" max="16" width="3.109375" customWidth="1"/>
+    <col min="17" max="33" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="G1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H1">
         <v>1</v>
@@ -492,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="L1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M1">
         <v>1</v>
@@ -558,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -580,8 +593,8 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>5</v>
+      <c r="H2" s="1">
+        <v>8</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -596,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -659,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -685,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -700,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -760,7 +773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -789,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -804,7 +817,7 @@
         <v>1</v>
       </c>
       <c r="O4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -861,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -893,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -908,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="P5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -962,12 +975,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -997,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -1063,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1071,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1101,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1164,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1205,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1265,7 +1278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1309,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1366,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1413,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1467,12 +1480,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1487,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1568,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1576,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1591,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1669,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1680,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1695,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1770,7 +1783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1784,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1799,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1871,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1888,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1903,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1972,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2031,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="T16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U16">
         <v>1</v>
@@ -2040,13 +2053,13 @@
         <v>1</v>
       </c>
       <c r="W16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X16">
         <v>1</v>
       </c>
       <c r="Y16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z16">
         <v>1</v>
@@ -2073,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2135,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="U17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V17">
         <v>1</v>
@@ -2144,7 +2157,7 @@
         <v>1</v>
       </c>
       <c r="X17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y17">
         <v>1</v>
@@ -2174,7 +2187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2248,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="Y18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z18">
         <v>1</v>
@@ -2275,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2325,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="Q19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2340,10 +2353,10 @@
         <v>1</v>
       </c>
       <c r="V19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X19">
         <v>1</v>
@@ -2376,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2429,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="R20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -2447,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="X20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y20">
         <v>1</v>
@@ -2477,7 +2490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2533,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="S21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T21">
         <v>1</v>
@@ -2551,7 +2564,7 @@
         <v>1</v>
       </c>
       <c r="Y21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z21">
         <v>1</v>
@@ -2578,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="Q22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R22">
         <v>1</v>
@@ -2637,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="T22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U22">
         <v>1</v>
@@ -2679,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>1</v>
       </c>
       <c r="R23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S23">
         <v>1</v>
@@ -2741,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="U23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V23">
         <v>1</v>
@@ -2780,7 +2793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2836,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="S24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T24">
         <v>1</v>
@@ -2845,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="V24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W24">
         <v>1</v>
@@ -2881,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2982,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3083,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3184,7 +3197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3285,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3386,7 +3399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3487,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3588,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -3691,7 +3704,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>